<commit_message>
renamed constants and added sample output files
</commit_message>
<xml_diff>
--- a/myFiles/portfolio_test.xlsx
+++ b/myFiles/portfolio_test.xlsx
@@ -13,7 +13,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>ticker</t>
+    <t>tickers</t>
   </si>
   <si>
     <t>shares</t>
@@ -71,10 +71,10 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
@@ -305,14 +305,14 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3">
@@ -322,7 +322,7 @@
       <c r="D2" s="4"/>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3">
@@ -332,14 +332,14 @@
       <c r="D3" s="4"/>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>25.0</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">

</xml_diff>